<commit_message>
Test plan updated with R2 goals
</commit_message>
<xml_diff>
--- a/Documents/testPlannerandTracker.xlsx
+++ b/Documents/testPlannerandTracker.xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
   <si>
     <t>Test Planner and Tracker</t>
   </si>
@@ -105,33 +113,50 @@
   </si>
   <si>
     <t>To be fixed before R2 with a randomize mechanism</t>
+  </si>
+  <si>
+    <t>Casual Questions</t>
+  </si>
+  <si>
+    <t>Big Red Button</t>
+  </si>
+  <si>
+    <t>Questions asked records</t>
+  </si>
+  <si>
+    <t>User asks questions unrelated to the site</t>
+  </si>
+  <si>
+    <t>Button to transfer to live chat with exec</t>
+  </si>
+  <si>
+    <t>Record questions asked in a log</t>
+  </si>
+  <si>
+    <t>Bot responds as required</t>
+  </si>
+  <si>
+    <t>Link to messenger chat</t>
+  </si>
+  <si>
+    <t>File with questions asked</t>
+  </si>
+  <si>
+    <t>not implemented</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -148,6 +173,12 @@
       <patternFill patternType="solid">
         <fgColor indexed="11"/>
         <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6600"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -302,101 +333,113 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+  </cellStyleXfs>
+  <cellXfs count="23">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-  </cellStyleXfs>
-  <cellXfs count="21">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium4"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ffff0000"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="000000D4"/>
+      <rgbColor rgb="00FCF305"/>
+      <rgbColor rgb="00F20884"/>
+      <rgbColor rgb="0000ABEA"/>
+      <rgbColor rgb="00900000"/>
+      <rgbColor rgb="00006411"/>
+      <rgbColor rgb="00000090"/>
+      <rgbColor rgb="0090713A"/>
+      <rgbColor rgb="004600A5"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="0063AAFE"/>
+      <rgbColor rgb="00DD2D32"/>
+      <rgbColor rgb="00FFF58C"/>
+      <rgbColor rgb="004EE257"/>
+      <rgbColor rgb="006711FF"/>
+      <rgbColor rgb="00FEA746"/>
+      <rgbColor rgb="00865357"/>
+      <rgbColor rgb="00A2BD90"/>
+      <rgbColor rgb="0063AAFE"/>
+      <rgbColor rgb="00DD2D32"/>
+      <rgbColor rgb="00FFF58C"/>
+      <rgbColor rgb="004EE257"/>
+      <rgbColor rgb="006711FF"/>
+      <rgbColor rgb="00FEA746"/>
+      <rgbColor rgb="00865357"/>
+      <rgbColor rgb="00A2BD90"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -528,7 +571,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -604,7 +647,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -623,7 +666,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -653,7 +696,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -679,7 +722,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -705,7 +748,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -731,7 +774,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -757,7 +800,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -783,7 +826,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -809,7 +852,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -835,7 +878,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -861,7 +904,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -874,9 +917,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -891,7 +940,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="20000" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="38000"/>
             </a:srgbClr>
@@ -899,7 +948,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -918,7 +967,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -944,7 +993,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -970,7 +1019,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -996,7 +1045,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1022,7 +1071,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1048,7 +1097,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1074,7 +1123,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1100,7 +1149,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1126,7 +1175,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1152,7 +1201,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1165,9 +1214,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1181,7 +1236,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1200,7 +1255,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1230,7 +1285,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1256,7 +1311,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1282,7 +1337,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1308,7 +1363,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1334,7 +1389,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1360,7 +1415,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1386,7 +1441,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1412,7 +1467,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1438,7 +1493,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1451,522 +1506,555 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:IV32"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D2" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="6.82031" style="1" customWidth="1"/>
-    <col min="2" max="2" width="39.4219" style="1" customWidth="1"/>
-    <col min="3" max="3" width="28.3516" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="39.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="28.33203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="40" style="1" customWidth="1"/>
-    <col min="5" max="5" width="32.7109" style="1" customWidth="1"/>
-    <col min="6" max="6" width="33.7734" style="1" customWidth="1"/>
+    <col min="5" max="5" width="32.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="33.83203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="39" style="1" customWidth="1"/>
-    <col min="8" max="8" width="23.3516" style="1" customWidth="1"/>
-    <col min="9" max="9" width="27.1719" style="1" customWidth="1"/>
+    <col min="8" max="8" width="23.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="27.1640625" style="1" customWidth="1"/>
     <col min="10" max="256" width="14.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.65" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:9" ht="13.75" customHeight="1">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" t="s" s="2">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s" s="2">
+      <c r="E1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-    </row>
-    <row r="2" ht="24.65" customHeight="1">
-      <c r="A2" t="s" s="6">
+      <c r="F1" s="20"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+    </row>
+    <row r="2" spans="1:9" ht="24.75" customHeight="1">
+      <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s" s="6">
+      <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s" s="5">
+      <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s" s="5">
+      <c r="D2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s" s="5">
+      <c r="E2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F2" t="s" s="6">
+      <c r="F2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G2" t="s" s="5">
+      <c r="G2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H2" t="s" s="6">
+      <c r="H2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I2" t="s" s="5">
+      <c r="I2" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" s="7">
+    <row r="3" spans="1:9" ht="13.75" customHeight="1">
+      <c r="A3" s="6">
         <v>1</v>
       </c>
-      <c r="B3" t="s" s="5">
+      <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" t="s" s="5">
+      <c r="C3" s="6"/>
+      <c r="D3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E3" t="s" s="5">
+      <c r="E3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F3" t="s" s="8">
+      <c r="F3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-    </row>
-    <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" s="9">
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+    </row>
+    <row r="4" spans="1:9" ht="13.75" customHeight="1">
+      <c r="A4" s="8">
         <v>2</v>
       </c>
-      <c r="B4" t="s" s="10">
+      <c r="B4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" t="s" s="10">
+      <c r="C4" s="8"/>
+      <c r="D4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E4" t="s" s="11">
+      <c r="E4" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F4" t="s" s="12">
+      <c r="F4" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="G4" t="s" s="13">
+      <c r="G4" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-    </row>
-    <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="14">
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+    </row>
+    <row r="5" spans="1:9" ht="13.75" customHeight="1">
+      <c r="A5" s="13">
         <v>3</v>
       </c>
-      <c r="B5" t="s" s="15">
+      <c r="B5" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="14"/>
-      <c r="D5" t="s" s="15">
+      <c r="C5" s="13"/>
+      <c r="D5" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="E5" t="s" s="16">
+      <c r="E5" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="F5" t="s" s="17">
+      <c r="F5" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G5" t="s" s="18">
+      <c r="G5" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-    </row>
-    <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="14">
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+    </row>
+    <row r="6" spans="1:9" ht="13.75" customHeight="1">
+      <c r="A6" s="13">
         <v>4</v>
       </c>
-      <c r="B6" t="s" s="15">
+      <c r="B6" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="14"/>
-      <c r="D6" t="s" s="15">
+      <c r="C6" s="13"/>
+      <c r="D6" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="E6" t="s" s="16">
+      <c r="E6" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="F6" t="s" s="17">
+      <c r="F6" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="G6" t="s" s="18">
+      <c r="G6" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-    </row>
-    <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="14">
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+    </row>
+    <row r="7" spans="1:9" ht="13.75" customHeight="1">
+      <c r="A7" s="13">
         <v>5</v>
       </c>
-      <c r="B7" t="s" s="15">
+      <c r="B7" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="14"/>
-      <c r="D7" t="s" s="15">
+      <c r="C7" s="13"/>
+      <c r="D7" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="E7" t="s" s="16">
+      <c r="E7" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="F7" t="s" s="19">
+      <c r="F7" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="G7" t="s" s="18">
+      <c r="G7" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-    </row>
-    <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="14">
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+    </row>
+    <row r="8" spans="1:9" ht="13.75" customHeight="1">
+      <c r="A8" s="13">
         <v>6</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-    </row>
-    <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="14">
+      <c r="B8" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+    </row>
+    <row r="9" spans="1:9" ht="13.75" customHeight="1">
+      <c r="A9" s="13">
         <v>7</v>
       </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-    </row>
-    <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="14">
+      <c r="B9" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+    </row>
+    <row r="10" spans="1:9" ht="13.75" customHeight="1">
+      <c r="A10" s="13">
         <v>8</v>
       </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-    </row>
-    <row r="11" ht="13.65" customHeight="1">
-      <c r="A11" s="14">
+      <c r="B10" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+    </row>
+    <row r="11" spans="1:9" ht="13.75" customHeight="1">
+      <c r="A11" s="13">
         <v>9</v>
       </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-    </row>
-    <row r="12" ht="13.65" customHeight="1">
-      <c r="A12" s="14">
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+    </row>
+    <row r="12" spans="1:9" ht="13.75" customHeight="1">
+      <c r="A12" s="13">
         <v>10</v>
       </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-    </row>
-    <row r="13" ht="13.65" customHeight="1">
-      <c r="A13" s="14">
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+    </row>
+    <row r="13" spans="1:9" ht="13.75" customHeight="1">
+      <c r="A13" s="13">
         <v>11</v>
       </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-    </row>
-    <row r="14" ht="13.65" customHeight="1">
-      <c r="A14" s="14">
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+    </row>
+    <row r="14" spans="1:9" ht="13.75" customHeight="1">
+      <c r="A14" s="13">
         <v>12</v>
       </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-    </row>
-    <row r="15" ht="13.65" customHeight="1">
-      <c r="A15" s="14">
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+    </row>
+    <row r="15" spans="1:9" ht="13.75" customHeight="1">
+      <c r="A15" s="13">
         <v>13</v>
       </c>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-    </row>
-    <row r="16" ht="13.65" customHeight="1">
-      <c r="A16" s="14">
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+    </row>
+    <row r="16" spans="1:9" ht="13.75" customHeight="1">
+      <c r="A16" s="13">
         <v>14</v>
       </c>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-    </row>
-    <row r="17" ht="13.65" customHeight="1">
-      <c r="A17" s="14">
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+    </row>
+    <row r="17" spans="1:9" ht="13.75" customHeight="1">
+      <c r="A17" s="13">
         <v>15</v>
       </c>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-    </row>
-    <row r="18" ht="13.65" customHeight="1">
-      <c r="A18" s="14">
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+    </row>
+    <row r="18" spans="1:9" ht="13.75" customHeight="1">
+      <c r="A18" s="13">
         <v>16</v>
       </c>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-    </row>
-    <row r="19" ht="13.65" customHeight="1">
-      <c r="A19" s="14">
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+    </row>
+    <row r="19" spans="1:9" ht="13.75" customHeight="1">
+      <c r="A19" s="13">
         <v>17</v>
       </c>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-    </row>
-    <row r="20" ht="13.65" customHeight="1">
-      <c r="A20" s="14">
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+    </row>
+    <row r="20" spans="1:9" ht="13.75" customHeight="1">
+      <c r="A20" s="13">
         <v>18</v>
       </c>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-    </row>
-    <row r="21" ht="13.65" customHeight="1">
-      <c r="A21" s="14">
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+    </row>
+    <row r="21" spans="1:9" ht="13.75" customHeight="1">
+      <c r="A21" s="13">
         <v>19</v>
       </c>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-    </row>
-    <row r="22" ht="13.65" customHeight="1">
-      <c r="A22" s="14">
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+    </row>
+    <row r="22" spans="1:9" ht="13.75" customHeight="1">
+      <c r="A22" s="13">
         <v>20</v>
       </c>
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-    </row>
-    <row r="23" ht="13.65" customHeight="1">
-      <c r="A23" s="14">
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+    </row>
+    <row r="23" spans="1:9" ht="13.75" customHeight="1">
+      <c r="A23" s="13">
         <v>21</v>
       </c>
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
-    </row>
-    <row r="24" ht="13.65" customHeight="1">
-      <c r="A24" s="14">
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+    </row>
+    <row r="24" spans="1:9" ht="13.75" customHeight="1">
+      <c r="A24" s="13">
         <v>22</v>
       </c>
-      <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
-    </row>
-    <row r="25" ht="13.65" customHeight="1">
-      <c r="A25" s="14">
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+    </row>
+    <row r="25" spans="1:9" ht="13.75" customHeight="1">
+      <c r="A25" s="13">
         <v>23</v>
       </c>
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="14"/>
-    </row>
-    <row r="26" ht="13.65" customHeight="1">
-      <c r="A26" s="14">
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+    </row>
+    <row r="26" spans="1:9" ht="13.75" customHeight="1">
+      <c r="A26" s="13">
         <v>24</v>
       </c>
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="14"/>
-    </row>
-    <row r="27" ht="13.65" customHeight="1">
-      <c r="A27" s="14">
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="13"/>
+    </row>
+    <row r="27" spans="1:9" ht="13.75" customHeight="1">
+      <c r="A27" s="13">
         <v>25</v>
       </c>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="14"/>
-    </row>
-    <row r="28" ht="13.65" customHeight="1">
-      <c r="A28" s="14">
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="13"/>
+    </row>
+    <row r="28" spans="1:9" ht="13.75" customHeight="1">
+      <c r="A28" s="13">
         <v>26</v>
       </c>
-      <c r="B28" s="14"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="14"/>
-    </row>
-    <row r="29" ht="13.65" customHeight="1">
-      <c r="A29" s="14">
+      <c r="B28" s="13"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="13"/>
+    </row>
+    <row r="29" spans="1:9" ht="13.75" customHeight="1">
+      <c r="A29" s="13">
         <v>27</v>
       </c>
-      <c r="B29" s="14"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="14"/>
-    </row>
-    <row r="30" ht="13.65" customHeight="1">
-      <c r="A30" s="14">
+      <c r="B29" s="13"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
+    </row>
+    <row r="30" spans="1:9" ht="13.75" customHeight="1">
+      <c r="A30" s="13">
         <v>28</v>
       </c>
-      <c r="B30" s="14"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
-      <c r="I30" s="14"/>
-    </row>
-    <row r="31" ht="13.65" customHeight="1">
-      <c r="A31" s="14">
+      <c r="B30" s="13"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="13"/>
+    </row>
+    <row r="31" spans="1:9" ht="13.75" customHeight="1">
+      <c r="A31" s="13">
         <v>29</v>
       </c>
-      <c r="B31" s="14"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="14"/>
-      <c r="I31" s="14"/>
-    </row>
-    <row r="32" ht="13.65" customHeight="1">
-      <c r="A32" s="14">
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="13"/>
+    </row>
+    <row r="32" spans="1:9" ht="13.75" customHeight="1">
+      <c r="A32" s="13">
         <v>30</v>
       </c>
-      <c r="B32" s="14"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
-      <c r="I32" s="14"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1974,9 +2062,13 @@
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>